<commit_message>
corrected a few data points
</commit_message>
<xml_diff>
--- a/TrevorHB.xlsx
+++ b/TrevorHB.xlsx
@@ -124,7 +124,7 @@
     <t xml:space="preserve">-22.5,6</t>
   </si>
   <si>
-    <t xml:space="preserve">-45,3,3,6</t>
+    <t xml:space="preserve">-45,3,3,6,5</t>
   </si>
   <si>
     <t xml:space="preserve">-25,4,5,8</t>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">-52.5,4,5,5</t>
   </si>
   <si>
-    <t xml:space="preserve">-27.5,6,3</t>
+    <t xml:space="preserve">-27.5,4,6,3</t>
   </si>
   <si>
     <t xml:space="preserve">-32.5,5,8</t>
@@ -389,10 +389,10 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -430,31 +430,31 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -462,31 +462,31 @@
       <c r="A3" s="1" t="n">
         <v>43767</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -494,31 +494,31 @@
       <c r="A4" s="1" t="n">
         <v>43770</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -526,7 +526,7 @@
       <c r="A5" s="1" t="n">
         <v>43773</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -558,31 +558,31 @@
       <c r="A6" s="1" t="n">
         <v>43776</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -590,31 +590,31 @@
       <c r="A7" s="1" t="n">
         <v>43779</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -622,31 +622,31 @@
       <c r="A8" s="1" t="n">
         <v>43782</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -654,31 +654,31 @@
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -686,7 +686,7 @@
       <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -718,31 +718,31 @@
       <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="J11" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -750,39 +750,39 @@
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="J12" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -811,354 +811,354 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J14" s="0" t="s">
+      <c r="J14" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="J15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J16" s="0" t="s">
+      <c r="J16" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="0" t="s">
+      <c r="G17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="H17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="I17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="0" t="s">
+      <c r="J17" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="0" t="s">
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="G18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="H18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="0" t="s">
+      <c r="I18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="0" t="s">
+      <c r="J18" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="0" t="s">
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="H19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="I19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J19" s="0" t="s">
+      <c r="J19" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="0" t="s">
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="G20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="0" t="s">
+      <c r="H20" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="I20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J20" s="0" t="s">
+      <c r="J20" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="0" t="s">
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="G21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="H21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="0" t="s">
+      <c r="J21" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="0" t="s">
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="G22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="0" t="s">
+      <c r="H22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="0" t="s">
+      <c r="I22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J22" s="0" t="s">
+      <c r="J22" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="0" t="s">
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="G23" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="H23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="I23" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="J23" s="0" t="s">
+      <c r="J23" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="0" t="s">
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="G24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H24" s="0" t="s">
+      <c r="H24" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="I24" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J24" s="0" t="s">
+      <c r="J24" s="2" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created quick error checker script for hangboard. Used this to fix two entries
</commit_message>
<xml_diff>
--- a/TrevorHB.xlsx
+++ b/TrevorHB.xlsx
@@ -430,7 +430,7 @@
     <t xml:space="preserve">-37.5,5,9</t>
   </si>
   <si>
-    <t xml:space="preserve">-22.5,9</t>
+    <t xml:space="preserve">-22.5,5,9</t>
   </si>
   <si>
     <t xml:space="preserve">-47.5,4,5,5</t>
@@ -457,7 +457,7 @@
     <t xml:space="preserve">-42.5,5,9</t>
   </si>
   <si>
-    <t xml:space="preserve">-32.5,7</t>
+    <t xml:space="preserve">-32.5,5,7</t>
   </si>
 </sst>
 </file>
@@ -566,10 +566,10 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K37" activeCellId="0" sqref="K37"/>
+      <selection pane="topLeft" activeCell="J37" activeCellId="0" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1436,7 +1436,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1660,7 +1660,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B35" s="2" t="s">

</xml_diff>

<commit_message>
update hangboard xlsx because I 'm impatient. slight change to error check
</commit_message>
<xml_diff>
--- a/TrevorHB.xlsx
+++ b/TrevorHB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="151">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -458,6 +458,21 @@
   </si>
   <si>
     <t xml:space="preserve">-32.5,5,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Feb 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-42.5,5,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-15,5,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-40,4,8,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-22.5,5,8</t>
   </si>
 </sst>
 </file>
@@ -563,13 +578,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J37" activeCellId="0" sqref="J37"/>
+      <selection pane="topLeft" activeCell="J38" activeCellId="0" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1753,6 +1768,38 @@
       </c>
       <c r="J37" s="2" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
had a good session, so uploading my local to see the progress
</commit_message>
<xml_diff>
--- a/TrevorHB.xlsx
+++ b/TrevorHB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="159">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -473,6 +473,30 @@
   </si>
   <si>
     <t xml:space="preserve">-22.5,5,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Mar 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-30,5,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-40,4,6,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Mar 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-40,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-22.5,3,7,7,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-37.5,4,9,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-20,5,7</t>
   </si>
 </sst>
 </file>
@@ -578,13 +602,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J38" activeCellId="0" sqref="J38"/>
+      <selection pane="topLeft" activeCell="J40" activeCellId="0" sqref="J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1771,7 +1795,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1800,6 +1824,70 @@
       </c>
       <c r="J38" s="2" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bouldering pushed to production + update hangboard progress
</commit_message>
<xml_diff>
--- a/TrevorHB.xlsx
+++ b/TrevorHB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="162">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -497,6 +497,15 @@
   </si>
   <si>
     <t xml:space="preserve">-20,5,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 Mar 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-7.5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-37.5,4,2,6</t>
   </si>
 </sst>
 </file>
@@ -602,13 +611,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J40" activeCellId="0" sqref="J40"/>
+      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1888,6 +1897,38 @@
       </c>
       <c r="J40" s="2" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add last 4 months of repeater data
</commit_message>
<xml_diff>
--- a/TrevorHB.xlsx
+++ b/TrevorHB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="231">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -506,6 +506,213 @@
   </si>
   <si>
     <t xml:space="preserve">-37.5,4,2,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Sep 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-27.5,2,7,5,6,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-10,3,7,5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-37.5,4,9,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-20,3,7,5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-27.5,3,7,6,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 Sep 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-32.5,3,7,5,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-17.5,5,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-42.5,4,9,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-25,4,7,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-32.5,4,6,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 Sep 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-42.5,3,5,6,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-25,5,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 Sep 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-32.5,3,7,6,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-17.5,3,9,6,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-42.5,4,6,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-32.5,4,8,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Oct 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-32.5,3,5,4,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-17.5,3,8,5,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-42.5,2,8,6,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-25,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-32.5,4,6,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 Oct 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-37.5,5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-47.5,5,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-30,4,6,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 Oct 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-37.5,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-30,3,7,8,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Nov 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-17.5,5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-37.5,4,4,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-45,4,7,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-27.5,4,7,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-30,3,5,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Nov 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-45,3,9,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-27.5,4,8,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-30,3,9,6,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 Nov 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-47.5,5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-20,3,9,7,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-45,2,8,7,4,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-27.5,4,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-30,4,5,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Nov 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-15,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-47.5,4,9,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-45,3,9,5,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-30,4,7,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Dec 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-47.5,5,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-37.5,3,8,6,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-45,4,6,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-30,3,9,4,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Dec 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-37.5,3,9,6,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-17.5,4,7,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-45,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-30,3,7,5,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 Dec 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-17.5,5,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-42.5,4,9,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-27.5,4,6,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-30,4,6,8</t>
   </si>
 </sst>
 </file>
@@ -514,7 +721,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD\ MMM\ YYYY"/>
+    <numFmt numFmtId="165" formatCode="dd\ mmm\ yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -607,17 +814,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H49" activeCellId="0" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1931,10 +2138,458 @@
         <v>31</v>
       </c>
     </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>